<commit_message>
8.1.2.9 and 8.1.3.0 See release notes for details
</commit_message>
<xml_diff>
--- a/WaterskiScoringSystem/WaterskiScoringSystem/IWWFRecordApplicationFormTemplate.xlsx
+++ b/WaterskiScoringSystem/WaterskiScoringSystem/IWWFRecordApplicationFormTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WaterskiScoring\GitHub\WaterskiScoringSystem\WaterskiScoringSystem\WaterskiScoringSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B171D70-417F-44A5-9964-4073D7E5A26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2653FA95-1DEE-4430-B6A2-96EAD39CD62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40320" yWindow="105" windowWidth="15555" windowHeight="15600" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32655" yWindow="1530" windowWidth="24855" windowHeight="14775" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID &amp; CERTIFICATION PAGE" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="221">
   <si>
     <t>FIRST PASS</t>
   </si>
@@ -437,9 +437,6 @@
   </si>
   <si>
     <t>COMMENTS</t>
-  </si>
-  <si>
-    <t>Note: Add any additional comments, explanation or data that will be of assistance in the independent verification o this pending record performance.</t>
   </si>
   <si>
     <t xml:space="preserve">         </t>
@@ -851,6 +848,45 @@
   </si>
   <si>
     <t xml:space="preserve">Setup files (grid &amp; check buoy, jump distance) </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> All AWSA NATIONAL Records are to be UPLOAD to ADRIVE.com https://www32.adrive.com/filemanager?dir=%2F
+LOG in under AWSATC@HOTMAIL.COM Password "Password34"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Add any additional comments, explanation or data that will be of assistance in the independent verification o this pending record performance.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1138,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1290,61 +1326,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1363,20 +1349,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1386,37 +1436,18 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1430,12 +1461,25 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1448,19 +1492,20 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1838,7 +1883,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1880,7 +1925,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1906,7 +1951,7 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
@@ -1920,140 +1965,140 @@
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="85" t="s">
-        <v>204</v>
-      </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
+      <c r="C1" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1">
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1">
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1">
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1">
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1">
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" spans="1:9" ht="17.649999999999999" customHeight="1">
       <c r="B8" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:9" ht="68.650000000000006" customHeight="1">
-      <c r="A9" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
+      <c r="A9" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
     </row>
     <row r="10" spans="1:9" ht="52.5" customHeight="1">
-      <c r="A10" s="87" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
+      <c r="A10" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1">
-      <c r="A11" s="87" t="s">
-        <v>193</v>
-      </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
+      <c r="A11" s="69" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
     </row>
     <row r="12" spans="1:9" ht="68.650000000000006" customHeight="1">
-      <c r="A12" s="87" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
+      <c r="A12" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
     </row>
     <row r="13" spans="1:9" ht="31.15" customHeight="1">
-      <c r="A13" s="87" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
+      <c r="A13" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
     </row>
     <row r="14" spans="1:9" ht="12" customHeight="1">
       <c r="A14" s="45"/>
@@ -2067,21 +2112,21 @@
       <c r="I14" s="44"/>
     </row>
     <row r="15" spans="1:9" ht="13.9" customHeight="1">
-      <c r="A15" s="83" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
+      <c r="A15" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2100,19 +2145,19 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A18" s="81" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
+      <c r="A18" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E18" s="56"/>
-      <c r="F18" s="81" t="s">
-        <v>195</v>
-      </c>
-      <c r="G18" s="82"/>
+      <c r="F18" s="62" t="s">
+        <v>194</v>
+      </c>
+      <c r="G18" s="63"/>
       <c r="H18" s="38"/>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" thickBot="1">
@@ -2125,15 +2170,15 @@
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="62" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
+      <c r="C20" s="85" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
       <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" thickBot="1">
@@ -2156,9 +2201,9 @@
       <c r="F22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="66"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="70"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="84"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A23" s="10"/>
@@ -2171,10 +2216,10 @@
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="69"/>
+        <v>155</v>
+      </c>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="27"/>
       <c r="F24" s="10" t="s">
         <v>43</v>
@@ -2192,17 +2237,17 @@
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A26" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="70"/>
+        <v>193</v>
+      </c>
+      <c r="B26" s="82"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="84"/>
       <c r="F26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="64"/>
-      <c r="H26" s="65"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="77"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A27" s="10"/>
@@ -2216,15 +2261,15 @@
       <c r="A28" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="65"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="77"/>
       <c r="F28" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G28" s="64"/>
-      <c r="H28" s="65"/>
+        <v>147</v>
+      </c>
+      <c r="G28" s="75"/>
+      <c r="H28" s="77"/>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A29" s="6"/>
@@ -2236,30 +2281,30 @@
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="78"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="79"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="64"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A31" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="65"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
       <c r="E31" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F31" s="74"/>
-      <c r="G31" s="65"/>
+        <v>157</v>
+      </c>
+      <c r="F31" s="80"/>
+      <c r="G31" s="77"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A32" s="10"/>
@@ -2272,16 +2317,16 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A33" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="65"/>
+        <v>153</v>
+      </c>
+      <c r="B33" s="81"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="77"/>
       <c r="E33" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F33" s="74"/>
-      <c r="G33" s="65"/>
+        <v>158</v>
+      </c>
+      <c r="F33" s="80"/>
+      <c r="G33" s="77"/>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="10"/>
@@ -2296,11 +2341,11 @@
       <c r="A35" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="65"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
       <c r="E35" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F35" s="36"/>
     </row>
@@ -2315,13 +2360,13 @@
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A37" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B37" s="64"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="65"/>
+        <v>154</v>
+      </c>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="77"/>
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:8" ht="18" customHeight="1" thickBot="1">
@@ -2335,10 +2380,10 @@
       <c r="H38" s="53"/>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1">
-      <c r="A39" s="80" t="s">
-        <v>147</v>
-      </c>
-      <c r="B39" s="79"/>
+      <c r="A39" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="64"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2356,11 +2401,11 @@
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A41" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+        <v>149</v>
+      </c>
+      <c r="B41" s="78"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="78"/>
       <c r="E41" s="22"/>
     </row>
     <row r="42" spans="1:8" ht="18" customHeight="1" thickBot="1">
@@ -2372,11 +2417,11 @@
     </row>
     <row r="43" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A43" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
+        <v>148</v>
+      </c>
+      <c r="B43" s="78"/>
+      <c r="C43" s="78"/>
+      <c r="D43" s="78"/>
       <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1">
@@ -2388,11 +2433,11 @@
     </row>
     <row r="45" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A45" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B45" s="71"/>
-      <c r="C45" s="71"/>
-      <c r="D45" s="71"/>
+        <v>150</v>
+      </c>
+      <c r="B45" s="78"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
       <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:8" ht="18" customHeight="1" thickBot="1">
@@ -2404,11 +2449,11 @@
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A47" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B47" s="71"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
+        <v>151</v>
+      </c>
+      <c r="B47" s="78"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="78"/>
       <c r="E47" s="22"/>
     </row>
     <row r="48" spans="1:8" ht="18" customHeight="1">
@@ -2422,8 +2467,8 @@
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:7" ht="18" customHeight="1">
-      <c r="A49" s="80"/>
-      <c r="B49" s="79"/>
+      <c r="A49" s="79"/>
+      <c r="B49" s="64"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="9"/>
@@ -2432,9 +2477,9 @@
     </row>
     <row r="50" spans="1:7" ht="18" customHeight="1">
       <c r="A50" s="10"/>
-      <c r="B50" s="76"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="76"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="72"/>
       <c r="E50" s="57"/>
     </row>
     <row r="51" spans="1:7" ht="18" customHeight="1">
@@ -2446,9 +2491,9 @@
     </row>
     <row r="52" spans="1:7" ht="18" customHeight="1">
       <c r="A52" s="10"/>
-      <c r="B52" s="76"/>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
+      <c r="B52" s="72"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72"/>
       <c r="E52" s="57"/>
     </row>
     <row r="53" spans="1:7" ht="18" customHeight="1">
@@ -2460,9 +2505,9 @@
     </row>
     <row r="54" spans="1:7" ht="18" customHeight="1">
       <c r="A54" s="10"/>
-      <c r="B54" s="76"/>
-      <c r="C54" s="76"/>
-      <c r="D54" s="76"/>
+      <c r="B54" s="72"/>
+      <c r="C54" s="72"/>
+      <c r="D54" s="72"/>
       <c r="E54" s="57"/>
     </row>
     <row r="55" spans="1:7" ht="18" customHeight="1">
@@ -2474,9 +2519,9 @@
     </row>
     <row r="56" spans="1:7" ht="18" customHeight="1">
       <c r="A56" s="10"/>
-      <c r="B56" s="76"/>
-      <c r="C56" s="76"/>
-      <c r="D56" s="76"/>
+      <c r="B56" s="72"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="72"/>
       <c r="E56" s="57"/>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1">
@@ -2488,9 +2533,9 @@
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1">
       <c r="A58" s="10"/>
-      <c r="B58" s="75"/>
-      <c r="C58" s="76"/>
-      <c r="D58" s="76"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72"/>
       <c r="E58" s="57"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1">
@@ -2503,9 +2548,9 @@
     </row>
     <row r="60" spans="1:7" ht="18" customHeight="1">
       <c r="A60" s="10"/>
-      <c r="B60" s="75"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="72"/>
+      <c r="D60" s="72"/>
       <c r="E60" s="27"/>
     </row>
     <row r="61" spans="1:7" ht="18" customHeight="1">
@@ -2513,9 +2558,9 @@
     </row>
     <row r="62" spans="1:7" ht="18" customHeight="1">
       <c r="A62" s="10"/>
-      <c r="B62" s="75"/>
-      <c r="C62" s="76"/>
-      <c r="D62" s="76"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="72"/>
+      <c r="D62" s="72"/>
       <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1">
@@ -2523,24 +2568,27 @@
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1">
       <c r="A64" s="10"/>
-      <c r="B64" s="75"/>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="72"/>
+      <c r="D64" s="72"/>
       <c r="E64" s="27"/>
     </row>
     <row r="65" ht="18" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="37">
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="C1:I7"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="A30:I30"/>
@@ -2557,18 +2605,15 @@
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="C1:I7"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A13:I13"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2604,19 +2649,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:14" ht="6.4" customHeight="1">
@@ -2638,161 +2683,161 @@
         <v>38</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="104" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="103" t="s">
+      <c r="C3" s="93" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="70"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="84"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="70"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="70"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="84"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="81" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="70"/>
+      <c r="A7" s="62" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="89"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="84"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A8" s="81" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="98"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="70"/>
+      <c r="A8" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="89"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="84"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A9" s="81" t="s">
-        <v>199</v>
-      </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="70"/>
+      <c r="A9" s="62" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="89"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="84"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A10" s="81" t="s">
-        <v>200</v>
-      </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="100"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="70"/>
+      <c r="A10" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="89"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="84"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A11" s="81" t="s">
-        <v>201</v>
-      </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="70"/>
+      <c r="A11" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="89"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="84"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -2812,56 +2857,56 @@
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="41"/>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="78"/>
+      <c r="H13" s="74"/>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
       <c r="K13" s="41"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A14" s="81" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="70"/>
+      <c r="A14" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="97"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="84"/>
       <c r="F14"/>
-      <c r="G14" s="81" t="s">
-        <v>187</v>
-      </c>
-      <c r="H14" s="92"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="70"/>
+      <c r="G14" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="H14" s="97"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="84"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A15" s="81" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="92"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="102"/>
+      <c r="A15" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="97"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="99"/>
       <c r="F15"/>
-      <c r="G15" s="81" t="s">
-        <v>188</v>
-      </c>
-      <c r="H15" s="92"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="70"/>
+      <c r="G15" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="H15" s="97"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="84"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
@@ -2928,7 +2973,7 @@
         <v>9.75</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18" customHeight="1" thickBot="1">
@@ -2945,7 +2990,7 @@
       <c r="I19" s="21"/>
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
-      <c r="L19" s="89"/>
+      <c r="L19" s="100"/>
     </row>
     <row r="20" spans="1:12" ht="18" customHeight="1" thickBot="1">
       <c r="A20" s="17" t="s">
@@ -2961,7 +3006,7 @@
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
-      <c r="L20" s="90"/>
+      <c r="L20" s="101"/>
     </row>
     <row r="21" spans="1:12" ht="18" customHeight="1" thickBot="1">
       <c r="A21" s="17" t="s">
@@ -2977,7 +3022,7 @@
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
-      <c r="L21" s="90"/>
+      <c r="L21" s="101"/>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1" thickBot="1">
       <c r="A22" s="17" t="s">
@@ -2993,7 +3038,7 @@
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
       <c r="K22" s="21"/>
-      <c r="L22" s="90"/>
+      <c r="L22" s="101"/>
     </row>
     <row r="23" spans="1:12" ht="18" customHeight="1" thickBot="1">
       <c r="A23" s="17" t="s">
@@ -3009,7 +3054,7 @@
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
-      <c r="L23" s="91"/>
+      <c r="L23" s="102"/>
     </row>
     <row r="24" spans="1:12" ht="10.5" customHeight="1">
       <c r="A24" s="6"/>
@@ -3248,28 +3293,28 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="1:13" ht="18" customHeight="1">
-      <c r="A38" s="95" t="s">
+      <c r="A38" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="78"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="78"/>
-      <c r="J38" s="78"/>
-      <c r="K38" s="78"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
       <c r="L38"/>
     </row>
     <row r="39" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="97"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>98</v>
@@ -3290,17 +3335,17 @@
         <v>103</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39" s="6"/>
     </row>
     <row r="40" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A40" s="93" t="s">
-        <v>189</v>
-      </c>
-      <c r="B40" s="94"/>
+      <c r="A40" s="95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" s="96"/>
       <c r="C40" s="19"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -3314,10 +3359,10 @@
       <c r="M40" s="6"/>
     </row>
     <row r="41" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A41" s="93" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="94"/>
+      <c r="A41" s="95" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="96"/>
       <c r="C41" s="19"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -3331,10 +3376,10 @@
       <c r="M41" s="6"/>
     </row>
     <row r="42" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A42" s="93" t="s">
-        <v>190</v>
-      </c>
-      <c r="B42" s="94"/>
+      <c r="A42" s="95" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" s="96"/>
       <c r="C42" s="19"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -3348,10 +3393,10 @@
       <c r="M42" s="6"/>
     </row>
     <row r="43" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="97"/>
+      <c r="B43" s="105"/>
       <c r="C43" s="15"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -3365,10 +3410,10 @@
       <c r="M43" s="6"/>
     </row>
     <row r="44" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A44" s="93" t="s">
-        <v>189</v>
-      </c>
-      <c r="B44" s="94"/>
+      <c r="A44" s="95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" s="96"/>
       <c r="C44" s="19"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -3382,10 +3427,10 @@
       <c r="M44" s="6"/>
     </row>
     <row r="45" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A45" s="93" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="94"/>
+      <c r="A45" s="95" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="96"/>
       <c r="C45" s="19"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
@@ -3399,10 +3444,10 @@
       <c r="M45" s="6"/>
     </row>
     <row r="46" spans="1:13" ht="18" customHeight="1" thickBot="1">
-      <c r="A46" s="93" t="s">
-        <v>190</v>
-      </c>
-      <c r="B46" s="94"/>
+      <c r="A46" s="95" t="s">
+        <v>189</v>
+      </c>
+      <c r="B46" s="96"/>
       <c r="C46" s="19"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -3426,18 +3471,18 @@
       <c r="A48" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="99" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="73"/>
-      <c r="J48" s="73"/>
-      <c r="K48" s="73"/>
+      <c r="B48" s="90" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="83"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="83"/>
+      <c r="J48" s="83"/>
+      <c r="K48" s="83"/>
       <c r="L48"/>
     </row>
     <row r="49" spans="1:12" ht="18" customHeight="1" thickBot="1">
@@ -11357,15 +11402,30 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L19:L23"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="B48:K48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="I6:K6"/>
@@ -11381,30 +11441,15 @@
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="B48:K48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="L19:L23"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -11441,16 +11486,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1">
       <c r="A2" s="2"/>
@@ -11467,176 +11512,176 @@
         <v>38</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="103" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="104" t="s">
+      <c r="C3" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="105"/>
+      <c r="H3" s="94"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="81" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="106"/>
+      <c r="A4" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="89"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="107"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="81" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="70"/>
+      <c r="A5" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="89"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="84"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A6" s="81" t="s">
-        <v>208</v>
-      </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="70"/>
+      <c r="A6" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="89"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="84"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="81" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="70"/>
+      <c r="A7" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="89"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="84"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A8" s="81" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" s="98"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="70"/>
+      <c r="A8" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="89"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="84"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A9" s="81" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="70"/>
+      <c r="A9" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="89"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A10" s="81" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="70"/>
+      <c r="A10" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="89"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="84"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A11" s="81" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="70"/>
+      <c r="A11" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="89"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="84"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A12" s="81" t="s">
-        <v>203</v>
-      </c>
-      <c r="B12" s="98"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="70"/>
+      <c r="A12" s="62" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="89"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="84"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A13" s="81" t="s">
-        <v>203</v>
-      </c>
-      <c r="B13" s="107"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="70"/>
+      <c r="A13" s="62" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="106"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="84"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -11657,58 +11702,58 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="41"/>
       <c r="D15" s="39"/>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="78"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="74"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="70"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="84"/>
       <c r="F16"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="79"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="64"/>
       <c r="I16" s="6"/>
       <c r="J16"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="92"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="102"/>
+      <c r="B17" s="97"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="99"/>
       <c r="F17"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="79"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="64"/>
       <c r="I17" s="6"/>
       <c r="J17"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="79"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18"/>
@@ -11721,12 +11766,12 @@
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A19" s="81" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="92"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="70"/>
+      <c r="A19" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="97"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="84"/>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" s="6"/>
@@ -11737,12 +11782,12 @@
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="92"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="70"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="84"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -12046,7 +12091,7 @@
     </row>
     <row r="45" spans="2:9" ht="18" customHeight="1" thickBot="1">
       <c r="B45" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="23"/>
@@ -12058,7 +12103,7 @@
     </row>
     <row r="46" spans="2:9" ht="18" customHeight="1" thickBot="1">
       <c r="B46" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="23"/>
@@ -12070,7 +12115,7 @@
     </row>
     <row r="47" spans="2:9" ht="18" customHeight="1" thickBot="1">
       <c r="B47" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="23"/>
@@ -12082,7 +12127,7 @@
     </row>
     <row r="48" spans="2:9" ht="18" customHeight="1" thickBot="1">
       <c r="B48" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="23"/>
@@ -12094,7 +12139,7 @@
     </row>
     <row r="49" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="B49" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="23"/>
@@ -12330,20 +12375,22 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="A18:B18"/>
@@ -12360,22 +12407,20 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -12408,119 +12453,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="103" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="120" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="121"/>
+      <c r="H3" s="116"/>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="89"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="107"/>
+    </row>
+    <row r="5" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A5" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="89"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="107"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A6" s="62" t="s">
         <v>161</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="106"/>
-    </row>
-    <row r="5" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="81" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="107"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A7" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="106"/>
-    </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A6" s="81" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="106"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="81" t="s">
+      <c r="B7" s="89"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="107"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A8" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="89"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="107"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A9" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="106"/>
-    </row>
-    <row r="8" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A8" s="81" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="107"/>
+    </row>
+    <row r="10" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A10" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B8" s="98"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="106"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A9" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="106"/>
-    </row>
-    <row r="10" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A10" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="106"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="107"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A11" s="6"/>
@@ -12531,79 +12576,79 @@
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="41"/>
       <c r="D12" s="39"/>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="117"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="78"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="97"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="62"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="64"/>
+    </row>
+    <row r="14" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A14" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="115" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="118" t="s">
         <v>168</v>
       </c>
-      <c r="F13" s="81"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="79"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A14" s="81" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="115" t="s">
-        <v>169</v>
-      </c>
-      <c r="F14" s="81"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="79"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="117"/>
+      <c r="J14" s="64"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A15" s="104"/>
-      <c r="B15" s="105"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="94"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
       <c r="F16" s="40"/>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" thickBot="1"/>
     <row r="18" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A18" s="81" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="98"/>
+      <c r="A18" s="62" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="89"/>
       <c r="C18" s="21"/>
       <c r="D18" s="6" t="s">
         <v>71</v>
@@ -12614,27 +12659,27 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A19" s="81" t="s">
-        <v>171</v>
-      </c>
-      <c r="B19" s="98"/>
+      <c r="A19" s="62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="89"/>
       <c r="C19" s="21"/>
       <c r="D19" s="6"/>
       <c r="E19" s="35"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="81" t="s">
-        <v>172</v>
-      </c>
-      <c r="B20" s="98"/>
+      <c r="A20" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="89"/>
       <c r="C20" s="21"/>
       <c r="D20" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H20" s="6"/>
     </row>
@@ -12647,71 +12692,71 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A22" s="118" t="s">
+      <c r="A22" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="118"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="119"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="114"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="114"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="98"/>
+      <c r="B23" s="89"/>
       <c r="C23" s="21"/>
       <c r="D23" s="10" t="s">
         <v>109</v>
       </c>
       <c r="E23" s="36"/>
       <c r="F23" s="54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1">
-      <c r="B24" s="108" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
+      <c r="B24" s="121" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A25" s="104"/>
-      <c r="B25" s="105"/>
+      <c r="A25" s="93"/>
+      <c r="B25" s="94"/>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A26" s="77" t="s">
-        <v>206</v>
-      </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
+      <c r="A26" s="73" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="74"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
       <c r="G26" s="49"/>
       <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A27" s="103" t="s">
+      <c r="A27" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="79"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="61"/>
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A28" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28"/>
       <c r="G28" s="9"/>
@@ -12743,16 +12788,16 @@
       <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1">
-      <c r="A31" s="112" t="s">
-        <v>174</v>
-      </c>
-      <c r="B31" s="116"/>
-      <c r="C31" s="116"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="116"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="116"/>
+      <c r="A31" s="110" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="111"/>
+      <c r="C31" s="111"/>
+      <c r="D31" s="111"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="111"/>
+      <c r="G31" s="111"/>
+      <c r="H31" s="111"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A32" s="32"/>
@@ -12765,16 +12810,16 @@
       <c r="H32" s="33"/>
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A33" s="81" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" s="107"/>
+      <c r="A33" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="B33" s="106"/>
       <c r="C33" s="37"/>
       <c r="D33"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="108"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
+      <c r="F33" s="121"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="6"/>
@@ -12783,16 +12828,16 @@
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:8" ht="18" customHeight="1">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="B35" s="110"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
+      <c r="B35" s="123"/>
+      <c r="C35" s="123"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="123"/>
     </row>
     <row r="36" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A36" s="3"/>
@@ -12810,9 +12855,9 @@
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="70"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="84"/>
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:8" ht="18" customHeight="1">
@@ -12826,19 +12871,19 @@
         <v>75</v>
       </c>
       <c r="B39" s="6"/>
-      <c r="C39" s="122" t="s">
-        <v>217</v>
-      </c>
-      <c r="D39" s="123"/>
+      <c r="C39" s="108" t="s">
+        <v>216</v>
+      </c>
+      <c r="D39" s="109"/>
       <c r="E39" s="3"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A40" s="81" t="s">
-        <v>176</v>
-      </c>
-      <c r="B40" s="92"/>
+      <c r="A40" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="B40" s="97"/>
       <c r="C40" s="9" t="s">
         <v>9</v>
       </c>
@@ -12851,10 +12896,10 @@
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A41" s="81" t="s">
-        <v>177</v>
-      </c>
-      <c r="B41" s="98"/>
+      <c r="A41" s="62" t="s">
+        <v>176</v>
+      </c>
+      <c r="B41" s="89"/>
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
       <c r="E41" s="6"/>
@@ -12863,10 +12908,10 @@
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A42" s="81" t="s">
-        <v>178</v>
-      </c>
-      <c r="B42" s="98"/>
+      <c r="A42" s="62" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" s="89"/>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
       <c r="E42" s="6"/>
@@ -12885,24 +12930,24 @@
         <v>74</v>
       </c>
       <c r="B44" s="6"/>
-      <c r="C44" s="122" t="s">
+      <c r="C44" s="108" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" s="109"/>
+      <c r="E44" s="79" t="s">
         <v>217</v>
       </c>
-      <c r="D44" s="123"/>
-      <c r="E44" s="80" t="s">
-        <v>218</v>
-      </c>
-      <c r="F44" s="79"/>
-      <c r="G44" s="122" t="s">
-        <v>217</v>
-      </c>
-      <c r="H44" s="123"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="108" t="s">
+        <v>216</v>
+      </c>
+      <c r="H44" s="109"/>
     </row>
     <row r="45" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A45" s="103" t="s">
+      <c r="A45" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="79"/>
+      <c r="B45" s="64"/>
       <c r="C45" s="9" t="s">
         <v>9</v>
       </c>
@@ -12921,8 +12966,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A46" s="103"/>
-      <c r="B46" s="109"/>
+      <c r="A46" s="92"/>
+      <c r="B46" s="122"/>
       <c r="C46" s="21">
         <v>0</v>
       </c>
@@ -12941,10 +12986,10 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A47" s="81" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" s="98"/>
+      <c r="A47" s="62" t="s">
+        <v>178</v>
+      </c>
+      <c r="B47" s="89"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
       <c r="E47" s="6"/>
@@ -12955,10 +13000,10 @@
       <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A48" s="81" t="s">
-        <v>180</v>
-      </c>
-      <c r="B48" s="98"/>
+      <c r="A48" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="89"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
       <c r="E48" s="6"/>
@@ -12969,29 +13014,29 @@
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A49" s="81" t="s">
-        <v>181</v>
-      </c>
-      <c r="B49" s="98"/>
+      <c r="A49" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="89"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A50" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="B50" s="98"/>
+      <c r="A50" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50" s="89"/>
       <c r="C50" s="21"/>
       <c r="D50" s="21"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
@@ -13003,20 +13048,20 @@
       <c r="G51" s="6"/>
     </row>
     <row r="52" spans="1:8" ht="18" customHeight="1">
-      <c r="A52" s="112" t="s">
+      <c r="A52" s="110" t="s">
         <v>120</v>
       </c>
-      <c r="B52" s="112"/>
-      <c r="C52" s="113"/>
-      <c r="D52" s="113"/>
-      <c r="E52" s="113"/>
-      <c r="F52" s="113"/>
-      <c r="G52" s="113"/>
-      <c r="H52" s="113"/>
+      <c r="B52" s="110"/>
+      <c r="C52" s="120"/>
+      <c r="D52" s="120"/>
+      <c r="E52" s="120"/>
+      <c r="F52" s="120"/>
+      <c r="G52" s="120"/>
+      <c r="H52" s="120"/>
     </row>
     <row r="53" spans="1:8" ht="18" customHeight="1">
       <c r="A53" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -13099,11 +13144,11 @@
       <c r="G58" s="6"/>
     </row>
     <row r="59" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A59" s="80" t="s">
+      <c r="A59" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="B59" s="79"/>
-      <c r="C59" s="79"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="64"/>
       <c r="D59" s="8"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -13168,21 +13213,55 @@
     </row>
     <row r="67" spans="1:6" ht="15">
       <c r="A67" s="10"/>
-      <c r="B67" s="111"/>
-      <c r="C67" s="111"/>
+      <c r="B67" s="119"/>
+      <c r="C67" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A52:H52"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="E12:F12"/>
@@ -13199,50 +13278,16 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A52:H52"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -13262,298 +13307,329 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E16"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12"/>
   <sheetData>
     <row r="1" spans="1:10" ht="25.15" customHeight="1">
-      <c r="A1" s="127" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
+      <c r="A1" s="131" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
     </row>
     <row r="2" spans="1:10" ht="15">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="125" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
     </row>
     <row r="3" spans="1:10" ht="20.25" thickBot="1">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="124" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="G3" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="92" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A5" s="92" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="108"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="G4" s="22"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A5" s="103" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
       <c r="G5" s="22"/>
-      <c r="H5" s="131" t="s">
+      <c r="H5" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="79"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="92" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
       <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A7" s="103" t="s">
-        <v>192</v>
-      </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
+      <c r="A7" s="92" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
       <c r="G7" s="22"/>
-      <c r="H7" s="131" t="s">
+      <c r="H7" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="79"/>
+      <c r="I7" s="64"/>
     </row>
     <row r="9" spans="1:10" ht="20.25" thickBot="1">
-      <c r="A9" s="128" t="s">
+      <c r="A9" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
       <c r="G9" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A10" s="103" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
+      <c r="A10" s="92" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="121"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
       <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
       <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
       <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
       <c r="G13" s="22"/>
     </row>
     <row r="15" spans="1:10" ht="20.25" thickBot="1">
-      <c r="A15" s="128" t="s">
+      <c r="A15" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
       <c r="G15" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A16" s="103" t="s">
+      <c r="A16" s="92" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A17" s="92" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="108"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A17" s="103" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="131" t="s">
+      <c r="H17" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="I17" s="79"/>
+      <c r="I17" s="64"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A18" s="103" t="s">
+      <c r="A18" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="131" t="s">
+      <c r="H18" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="I18" s="79"/>
+      <c r="I18" s="64"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A19" s="103" t="s">
+      <c r="A19" s="92" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="131" t="s">
+      <c r="H19" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="I19" s="79"/>
+      <c r="I19" s="64"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A20" s="103" t="s">
-        <v>219</v>
-      </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
+      <c r="A20" s="92" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="131" t="s">
+      <c r="H20" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="I20" s="79"/>
+      <c r="I20" s="64"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A21" s="103" t="s">
+      <c r="A21" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="79"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="131" t="s">
+      <c r="H21" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="I21" s="79"/>
+      <c r="I21" s="64"/>
     </row>
     <row r="22" spans="1:11" ht="15">
       <c r="A22" s="6"/>
       <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:11" ht="19.5">
-      <c r="A23" s="128" t="s">
+      <c r="A23" s="124" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="79"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
       <c r="G23" s="27"/>
     </row>
-    <row r="24" spans="1:11" s="31" customFormat="1" ht="27.4" customHeight="1" thickBot="1">
-      <c r="A24" s="129" t="s">
-        <v>129</v>
-      </c>
-      <c r="B24" s="130"/>
-      <c r="C24" s="130"/>
-      <c r="D24" s="130"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
-      <c r="G24" s="130"/>
-      <c r="H24" s="130"/>
-      <c r="I24" s="130"/>
-      <c r="J24" s="130"/>
-    </row>
-    <row r="25" spans="1:11" ht="136.9" customHeight="1" thickBot="1">
-      <c r="A25" s="124"/>
-      <c r="B25" s="125"/>
-      <c r="C25" s="125"/>
-      <c r="D25" s="125"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="125"/>
-      <c r="G25" s="125"/>
-      <c r="H25" s="125"/>
-      <c r="I25" s="125"/>
-      <c r="J25" s="125"/>
-      <c r="K25" s="126"/>
-    </row>
-    <row r="26" spans="1:11" ht="15">
-      <c r="A26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1"/>
-    <row r="28" spans="1:11" ht="15">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1">
+    <row r="24" spans="1:11" ht="50.1" customHeight="1">
+      <c r="A24" s="134" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" s="135"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="135"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="136"/>
+      <c r="K24" s="136"/>
+    </row>
+    <row r="25" spans="1:11" s="31" customFormat="1" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A25" s="132" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" s="133"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="133"/>
+      <c r="H25" s="133"/>
+      <c r="I25" s="133"/>
+      <c r="J25" s="133"/>
+    </row>
+    <row r="26" spans="1:11" ht="136.9" customHeight="1" thickBot="1">
+      <c r="A26" s="128"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
+      <c r="K26" s="130"/>
+    </row>
+    <row r="27" spans="1:11" ht="15">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1"/>
+    <row r="29" spans="1:11" ht="15">
       <c r="A29" s="6"/>
     </row>
+    <row r="30" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A30" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A2:I2"/>
@@ -13568,21 +13644,6 @@
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>